<commit_message>
Add new climb/descent fuel system
</commit_message>
<xml_diff>
--- a/v2/descent-fuel-performance.xlsx
+++ b/v2/descent-fuel-performance.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattmaring/Documents/GitHub/A320-family-fuel-model/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E92C5F-D0EB-D347-97B8-B7F64C0FA684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA65AD2D-E8EB-9F45-9B2A-BE156FF834C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="500" windowWidth="15660" windowHeight="16640" xr2:uid="{F4057D04-69D9-6541-9B9E-A2BC0BA45835}"/>
+    <workbookView xWindow="9680" yWindow="500" windowWidth="19120" windowHeight="16640" xr2:uid="{F4057D04-69D9-6541-9B9E-A2BC0BA45835}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="descent" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="14">
   <si>
     <t>FL</t>
   </si>
@@ -63,6 +67,18 @@
   </si>
   <si>
     <t>WEIGHT (LBS)</t>
+  </si>
+  <si>
+    <t>Sum of TIME (MIN)</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -98,8 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +136,1228 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="44262.641248842592" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="90" xr:uid="{DE28D427-A41E-7944-88E0-1FBE0A547C2E}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:I91" sheet="descent"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="FL" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="15" maxValue="390" count="18">
+        <n v="15"/>
+        <n v="50"/>
+        <n v="100"/>
+        <n v="120"/>
+        <n v="140"/>
+        <n v="160"/>
+        <n v="180"/>
+        <n v="200"/>
+        <n v="220"/>
+        <n v="240"/>
+        <n v="250"/>
+        <n v="270"/>
+        <n v="290"/>
+        <n v="310"/>
+        <n v="330"/>
+        <n v="350"/>
+        <n v="370"/>
+        <n v="390"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="WEIGHT (LBS)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="99.208017990000002" maxValue="143.30047042999999" count="5">
+        <n v="99.208017990000002"/>
+        <n v="110.2311311"/>
+        <n v="121.25424421"/>
+        <n v="132.27735731999999"/>
+        <n v="143.30047042999999"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="WEIGHT (KG)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="45" maxValue="65" count="5">
+        <n v="45"/>
+        <n v="50"/>
+        <n v="55"/>
+        <n v="60"/>
+        <n v="65"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="TIME (MIN)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="17.399999999999999"/>
+    </cacheField>
+    <cacheField name="FUEL (KG)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="204"/>
+    </cacheField>
+    <cacheField name="FUEL (LBS)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="449.74247999999994"/>
+    </cacheField>
+    <cacheField name="DIST (NM)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="106"/>
+    </cacheField>
+    <cacheField name="N1" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="68.8" maxValue="72.099999999999994"/>
+    </cacheField>
+    <cacheField name="IAS (KT)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="241" maxValue="300"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="90">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.7"/>
+    <n v="15"/>
+    <n v="33.069299999999998"/>
+    <n v="7"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1.7999999999999998"/>
+    <n v="15.75"/>
+    <n v="34.722764999999995"/>
+    <n v="7.5"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="1.9"/>
+    <n v="16.5"/>
+    <n v="36.37623"/>
+    <n v="8"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="2"/>
+    <n v="17.25"/>
+    <n v="38.029694999999997"/>
+    <n v="8.5"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="2.1"/>
+    <n v="18"/>
+    <n v="39.683159999999994"/>
+    <n v="9"/>
+    <s v="IDLE"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.9000000000000004"/>
+    <n v="48"/>
+    <n v="105.82175999999998"/>
+    <n v="23"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="5.1750000000000007"/>
+    <n v="50.5"/>
+    <n v="111.33330999999998"/>
+    <n v="24.25"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="5.45"/>
+    <n v="53"/>
+    <n v="116.84485999999998"/>
+    <n v="25.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.6"/>
+    <n v="57"/>
+    <n v="125.66333999999999"/>
+    <n v="27"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="5.7249999999999996"/>
+    <n v="55.5"/>
+    <n v="122.35640999999998"/>
+    <n v="26.75"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="5.9249999999999998"/>
+    <n v="60.25"/>
+    <n v="132.82835499999999"/>
+    <n v="28.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="6"/>
+    <n v="58"/>
+    <n v="127.86795999999998"/>
+    <n v="28"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="6.25"/>
+    <n v="63.5"/>
+    <n v="139.99337"/>
+    <n v="30"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.3"/>
+    <n v="67"/>
+    <n v="147.70953999999998"/>
+    <n v="31"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="6.5750000000000002"/>
+    <n v="66.75"/>
+    <n v="147.15838499999998"/>
+    <n v="31.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="6.6999999999999993"/>
+    <n v="71"/>
+    <n v="156.52802"/>
+    <n v="33"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="6.9"/>
+    <n v="70"/>
+    <n v="154.32339999999999"/>
+    <n v="33"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="7.1"/>
+    <n v="75"/>
+    <n v="165.34649999999999"/>
+    <n v="35"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.1"/>
+    <n v="78"/>
+    <n v="171.96035999999998"/>
+    <n v="36"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="7.5"/>
+    <n v="79"/>
+    <n v="174.16497999999999"/>
+    <n v="37"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="7.5250000000000004"/>
+    <n v="82.75"/>
+    <n v="182.43230499999999"/>
+    <n v="38.25"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.8"/>
+    <n v="86"/>
+    <n v="189.59732"/>
+    <n v="40"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="7.9"/>
+    <n v="83"/>
+    <n v="182.98345999999998"/>
+    <n v="39"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="7.95"/>
+    <n v="87.5"/>
+    <n v="192.90424999999999"/>
+    <n v="40.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="8.3000000000000007"/>
+    <n v="91.75"/>
+    <n v="202.27388499999998"/>
+    <n v="42.75"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="8.375"/>
+    <n v="92.25"/>
+    <n v="203.376195"/>
+    <n v="42.75"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="8.5"/>
+    <n v="94"/>
+    <n v="207.23427999999998"/>
+    <n v="45"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="8.8000000000000007"/>
+    <n v="97"/>
+    <n v="213.84813999999997"/>
+    <n v="45"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="8.8000000000000007"/>
+    <n v="97.5"/>
+    <n v="214.95044999999999"/>
+    <n v="45.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="9.0250000000000004"/>
+    <n v="100.25"/>
+    <n v="221.01315499999998"/>
+    <n v="47.75"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9.1"/>
+    <n v="100"/>
+    <n v="220.46199999999999"/>
+    <n v="49"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="9.3000000000000007"/>
+    <n v="103.25"/>
+    <n v="227.62701499999997"/>
+    <n v="48.25"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="9.5500000000000007"/>
+    <n v="106.5"/>
+    <n v="234.79202999999998"/>
+    <n v="50.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="9.6999999999999993"/>
+    <n v="106.75"/>
+    <n v="235.34318499999998"/>
+    <n v="52.25"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9.6999999999999993"/>
+    <n v="105"/>
+    <n v="231.48509999999999"/>
+    <n v="53"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="9.8000000000000007"/>
+    <n v="109"/>
+    <n v="240.30357999999998"/>
+    <n v="51"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10"/>
+    <n v="107"/>
+    <n v="235.89433999999997"/>
+    <n v="55"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="10.074999999999999"/>
+    <n v="112.75"/>
+    <n v="248.57090499999998"/>
+    <n v="53.25"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="10.3"/>
+    <n v="113.5"/>
+    <n v="250.22436999999996"/>
+    <n v="55.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="10.35"/>
+    <n v="112"/>
+    <n v="246.91743999999997"/>
+    <n v="56.75"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="10.6"/>
+    <n v="119"/>
+    <n v="262.34977999999995"/>
+    <n v="56"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10.6"/>
+    <n v="110"/>
+    <n v="242.50819999999999"/>
+    <n v="59"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="10.675000000000001"/>
+    <n v="114.25"/>
+    <n v="251.87783499999998"/>
+    <n v="59"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="10.9"/>
+    <n v="120.25"/>
+    <n v="265.10555499999998"/>
+    <n v="58.75"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="11"/>
+    <n v="119"/>
+    <n v="262.34977999999995"/>
+    <n v="60.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="11.1"/>
+    <n v="114"/>
+    <n v="251.32667999999998"/>
+    <n v="64"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="11.3"/>
+    <n v="117.75"/>
+    <n v="259.59400499999998"/>
+    <n v="63.25"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="11.35"/>
+    <n v="121.5"/>
+    <n v="267.86132999999995"/>
+    <n v="63"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="11.5"/>
+    <n v="127"/>
+    <n v="279.98674"/>
+    <n v="62"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="11.6"/>
+    <n v="117"/>
+    <n v="257.94054"/>
+    <n v="67"/>
+    <s v="IDLE"/>
+    <n v="289"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="11.65"/>
+    <n v="126"/>
+    <n v="277.78211999999996"/>
+    <n v="64.25"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="11.875"/>
+    <n v="121.75"/>
+    <n v="268.412485"/>
+    <n v="68.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="12"/>
+    <n v="125.5"/>
+    <n v="276.67980999999997"/>
+    <n v="67.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="12"/>
+    <n v="119"/>
+    <n v="262.34977999999995"/>
+    <n v="70"/>
+    <s v="IDLE"/>
+    <n v="277"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="12.024999999999999"/>
+    <n v="128.75"/>
+    <n v="283.84482499999996"/>
+    <n v="67"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="12.3"/>
+    <n v="133"/>
+    <n v="293.21445999999997"/>
+    <n v="68"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="12.399999999999999"/>
+    <n v="125"/>
+    <n v="275.57749999999999"/>
+    <n v="71.75"/>
+    <s v="IDLE"/>
+    <n v="289"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="12.649999999999999"/>
+    <n v="129.5"/>
+    <n v="285.49829"/>
+    <n v="73"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="12.7"/>
+    <n v="136"/>
+    <n v="299.82831999999996"/>
+    <n v="71"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="12.7"/>
+    <n v="133.25"/>
+    <n v="293.76561499999997"/>
+    <n v="71.75"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="12.85"/>
+    <n v="127.5"/>
+    <n v="281.08904999999999"/>
+    <n v="75.25"/>
+    <s v="IDLE"/>
+    <n v="277"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="12.9"/>
+    <n v="134"/>
+    <n v="295.41907999999995"/>
+    <n v="77"/>
+    <n v="72.099999999999994"/>
+    <n v="264"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="13.2"/>
+    <n v="133"/>
+    <n v="293.21445999999997"/>
+    <n v="76.5"/>
+    <s v="IDLE"/>
+    <n v="289"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="13.4"/>
+    <n v="141"/>
+    <n v="310.85141999999996"/>
+    <n v="76"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="13.424999999999999"/>
+    <n v="137.25"/>
+    <n v="302.58409499999999"/>
+    <n v="77.5"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="13.675000000000001"/>
+    <n v="139.5"/>
+    <n v="307.54449"/>
+    <n v="81.5"/>
+    <s v="IDLE"/>
+    <n v="264"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="13.7"/>
+    <n v="136"/>
+    <n v="299.82831999999996"/>
+    <n v="80.5"/>
+    <s v="IDLE"/>
+    <n v="277"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="14"/>
+    <n v="141"/>
+    <n v="310.85141999999996"/>
+    <n v="81.25"/>
+    <s v="IDLE"/>
+    <n v="289"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="14.2"/>
+    <n v="145"/>
+    <n v="319.66989999999998"/>
+    <n v="82"/>
+    <s v="IDLE"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="14.45"/>
+    <n v="145"/>
+    <n v="319.66989999999998"/>
+    <n v="86"/>
+    <s v="IDLE"/>
+    <n v="264"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="14.55"/>
+    <n v="144.5"/>
+    <n v="318.56759"/>
+    <n v="85.75"/>
+    <s v="IDLE"/>
+    <n v="277"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="14.6"/>
+    <n v="174"/>
+    <n v="383.60387999999995"/>
+    <n v="89"/>
+    <n v="69.900000000000006"/>
+    <n v="252"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="14.8"/>
+    <n v="149"/>
+    <n v="328.48837999999995"/>
+    <n v="86"/>
+    <s v="IDLE"/>
+    <n v="289"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="15.125"/>
+    <n v="170.5"/>
+    <n v="375.88770999999997"/>
+    <n v="91.75"/>
+    <n v="72.099999999999994"/>
+    <n v="252"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="15.225"/>
+    <n v="150.5"/>
+    <n v="331.79530999999997"/>
+    <n v="90.5"/>
+    <s v="IDLE"/>
+    <n v="264"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="15.4"/>
+    <n v="153"/>
+    <n v="337.30685999999997"/>
+    <n v="91"/>
+    <s v="IDLE"/>
+    <n v="277"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="15.649999999999999"/>
+    <n v="167"/>
+    <n v="368.17153999999999"/>
+    <n v="94.5"/>
+    <s v="IDLE"/>
+    <n v="252"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="16"/>
+    <n v="156"/>
+    <n v="343.92071999999996"/>
+    <n v="95"/>
+    <s v="IDLE"/>
+    <n v="264"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.100000000000001"/>
+    <n v="204"/>
+    <n v="449.74247999999994"/>
+    <n v="101"/>
+    <n v="68.8"/>
+    <n v="241"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="16.174999999999997"/>
+    <n v="163.5"/>
+    <n v="360.45536999999996"/>
+    <n v="97.25"/>
+    <s v="IDLE"/>
+    <n v="252"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="16.425000000000001"/>
+    <n v="194.25"/>
+    <n v="428.24743499999994"/>
+    <n v="102.25"/>
+    <n v="69.900000000000006"/>
+    <n v="241"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="16.7"/>
+    <n v="160"/>
+    <n v="352.73919999999998"/>
+    <n v="100"/>
+    <s v="IDLE"/>
+    <n v="252"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="16.75"/>
+    <n v="184.5"/>
+    <n v="406.75238999999999"/>
+    <n v="103.5"/>
+    <n v="72.099999999999994"/>
+    <n v="241"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="17.074999999999999"/>
+    <n v="174.75"/>
+    <n v="385.25734499999999"/>
+    <n v="104.75"/>
+    <s v="IDLE"/>
+    <n v="241"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="17.399999999999999"/>
+    <n v="165"/>
+    <n v="363.76229999999998"/>
+    <n v="106"/>
+    <s v="IDLE"/>
+    <n v="241"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8A7F99EB-0C12-9F44-B1CF-750CE9F84891}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="19">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of TIME (MIN)" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,11 +1676,502 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8037D066-B8B3-A841-9A81-FC34D367BC20}">
+  <dimension ref="A3:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>55</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>100</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5.1750000000000007</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5.45</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5.7249999999999996</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3">
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>120</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5.9249999999999998</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6.5750000000000002</v>
+      </c>
+      <c r="F8" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="G8" s="3">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>140</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>6.6999999999999993</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="G9" s="3">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>160</v>
+      </c>
+      <c r="B10" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.5250000000000004</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7.95</v>
+      </c>
+      <c r="E10" s="3">
+        <v>8.375</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G10" s="3">
+        <v>39.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>180</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D11" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E11" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F11" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G11" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>200</v>
+      </c>
+      <c r="B12" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>9.0250000000000004</v>
+      </c>
+      <c r="D12" s="3">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10.074999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <v>10.6</v>
+      </c>
+      <c r="G12" s="3">
+        <v>47.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>220</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10.9</v>
+      </c>
+      <c r="F13" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="G13" s="3">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>240</v>
+      </c>
+      <c r="B14" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C14" s="3">
+        <v>10.35</v>
+      </c>
+      <c r="D14" s="3">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3">
+        <v>11.65</v>
+      </c>
+      <c r="F14" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="G14" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>250</v>
+      </c>
+      <c r="B15" s="3">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3">
+        <v>10.675000000000001</v>
+      </c>
+      <c r="D15" s="3">
+        <v>11.35</v>
+      </c>
+      <c r="E15" s="3">
+        <v>12.024999999999999</v>
+      </c>
+      <c r="F15" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="G15" s="3">
+        <v>56.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>270</v>
+      </c>
+      <c r="B16" s="3">
+        <v>10.6</v>
+      </c>
+      <c r="C16" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="F16" s="3">
+        <v>13.4</v>
+      </c>
+      <c r="G16" s="3">
+        <v>59.999999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>290</v>
+      </c>
+      <c r="B17" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>11.875</v>
+      </c>
+      <c r="D17" s="3">
+        <v>12.649999999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>13.424999999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="G17" s="3">
+        <v>63.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>310</v>
+      </c>
+      <c r="B18" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="C18" s="3">
+        <v>12.399999999999999</v>
+      </c>
+      <c r="D18" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>14</v>
+      </c>
+      <c r="F18" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="G18" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>330</v>
+      </c>
+      <c r="B19" s="3">
+        <v>12</v>
+      </c>
+      <c r="C19" s="3">
+        <v>12.85</v>
+      </c>
+      <c r="D19" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="E19" s="3">
+        <v>14.55</v>
+      </c>
+      <c r="F19" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="G19" s="3">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>350</v>
+      </c>
+      <c r="B20" s="3">
+        <v>12.9</v>
+      </c>
+      <c r="C20" s="3">
+        <v>13.675000000000001</v>
+      </c>
+      <c r="D20" s="3">
+        <v>14.45</v>
+      </c>
+      <c r="E20" s="3">
+        <v>15.225</v>
+      </c>
+      <c r="F20" s="3">
+        <v>16</v>
+      </c>
+      <c r="G20" s="3">
+        <v>72.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>370</v>
+      </c>
+      <c r="B21" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="C21" s="3">
+        <v>15.125</v>
+      </c>
+      <c r="D21" s="3">
+        <v>15.649999999999999</v>
+      </c>
+      <c r="E21" s="3">
+        <v>16.174999999999997</v>
+      </c>
+      <c r="F21" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="G21" s="3">
+        <v>78.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>390</v>
+      </c>
+      <c r="B22" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C22" s="3">
+        <v>16.425000000000001</v>
+      </c>
+      <c r="D22" s="3">
+        <v>16.75</v>
+      </c>
+      <c r="E22" s="3">
+        <v>17.074999999999999</v>
+      </c>
+      <c r="F22" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G22" s="3">
+        <v>83.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3">
+        <v>159.59999999999997</v>
+      </c>
+      <c r="C23" s="3">
+        <v>168.82499999999999</v>
+      </c>
+      <c r="D23" s="3">
+        <v>178.04999999999998</v>
+      </c>
+      <c r="E23" s="3">
+        <v>187.27499999999998</v>
+      </c>
+      <c r="F23" s="3">
+        <v>196.50000000000003</v>
+      </c>
+      <c r="G23" s="3">
+        <v>890.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1D37F7-26A0-AD47-B821-48DF634ABCCC}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +2219,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>390</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>99.208017990000002</v>
@@ -494,143 +2228,143 @@
         <v>45</v>
       </c>
       <c r="D2">
-        <v>16.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>204</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>449.74247999999994</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>101</v>
-      </c>
-      <c r="H2">
-        <v>68.8</v>
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>370</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>99.208017990000002</v>
+        <v>110.2311311</v>
       </c>
       <c r="C3">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>14.6</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>383.60387999999995</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>89</v>
-      </c>
-      <c r="H3">
-        <v>69.900000000000006</v>
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>350</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>99.208017990000002</v>
+        <v>121.25424421</v>
       </c>
       <c r="C4">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>295.41907999999995</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>77</v>
-      </c>
-      <c r="H4">
-        <v>72.099999999999994</v>
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>330</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>99.208017990000002</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C5">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>262.34977999999995</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="H5" t="s">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>277</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>310</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>99.208017990000002</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C6">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D6">
-        <v>11.6</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>257.94054</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>289</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>290</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>99.208017990000002</v>
@@ -639,143 +2373,143 @@
         <v>45</v>
       </c>
       <c r="D7">
-        <v>11.1</v>
+        <v>1.7</v>
       </c>
       <c r="E7">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="F7">
-        <v>251.32667999999998</v>
+        <v>33.069299999999998</v>
       </c>
       <c r="G7">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>270</v>
+        <v>50</v>
       </c>
       <c r="B8">
-        <v>99.208017990000002</v>
+        <v>110.2311311</v>
       </c>
       <c r="C8">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D8">
-        <v>10.6</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="E8">
-        <v>110</v>
+        <v>15.75</v>
       </c>
       <c r="F8">
-        <v>242.50819999999999</v>
+        <v>34.722764999999995</v>
       </c>
       <c r="G8">
-        <v>59</v>
+        <v>7.5</v>
       </c>
       <c r="H8" t="s">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>121.25424421</v>
+      </c>
+      <c r="C9">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <v>1.9</v>
+      </c>
+      <c r="E9">
+        <v>16.5</v>
+      </c>
+      <c r="F9">
+        <v>36.37623</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>250</v>
-      </c>
-      <c r="B9">
-        <v>99.208017990000002</v>
-      </c>
-      <c r="C9">
-        <v>45</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>107</v>
-      </c>
-      <c r="F9">
-        <v>235.89433999999997</v>
-      </c>
-      <c r="G9">
-        <v>55</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>240</v>
+        <v>50</v>
       </c>
       <c r="B10">
-        <v>99.208017990000002</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C10">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <v>9.6999999999999993</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>105</v>
+        <v>17.25</v>
       </c>
       <c r="F10">
-        <v>231.48509999999999</v>
+        <v>38.029694999999997</v>
       </c>
       <c r="G10">
-        <v>53</v>
+        <v>8.5</v>
       </c>
       <c r="H10" t="s">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>220</v>
+        <v>50</v>
       </c>
       <c r="B11">
-        <v>99.208017990000002</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C11">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D11">
-        <v>9.1</v>
+        <v>2.1</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="F11">
-        <v>220.46199999999999</v>
+        <v>39.683159999999994</v>
       </c>
       <c r="G11">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s">
         <v>1</v>
       </c>
       <c r="I11">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B12">
         <v>99.208017990000002</v>
@@ -784,16 +2518,16 @@
         <v>45</v>
       </c>
       <c r="D12">
-        <v>8.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E12">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="F12">
-        <v>207.23427999999998</v>
+        <v>105.82175999999998</v>
       </c>
       <c r="G12">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s">
         <v>1</v>
@@ -804,25 +2538,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="B13">
-        <v>99.208017990000002</v>
+        <v>110.2311311</v>
       </c>
       <c r="C13">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D13">
-        <v>7.8</v>
+        <v>5.1750000000000007</v>
       </c>
       <c r="E13">
-        <v>86</v>
+        <v>50.5</v>
       </c>
       <c r="F13">
-        <v>189.59732</v>
+        <v>111.33330999999998</v>
       </c>
       <c r="G13">
-        <v>40</v>
+        <v>24.25</v>
       </c>
       <c r="H13" t="s">
         <v>1</v>
@@ -833,25 +2567,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="B14">
-        <v>99.208017990000002</v>
+        <v>121.25424421</v>
       </c>
       <c r="C14">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D14">
-        <v>7.1</v>
+        <v>5.45</v>
       </c>
       <c r="E14">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="F14">
-        <v>171.96035999999998</v>
+        <v>116.84485999999998</v>
       </c>
       <c r="G14">
-        <v>36</v>
+        <v>25.5</v>
       </c>
       <c r="H14" t="s">
         <v>1</v>
@@ -862,7 +2596,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B15">
         <v>99.208017990000002</v>
@@ -871,16 +2605,16 @@
         <v>45</v>
       </c>
       <c r="D15">
-        <v>6.3</v>
+        <v>5.6</v>
       </c>
       <c r="E15">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F15">
-        <v>147.70953999999998</v>
+        <v>125.66333999999999</v>
       </c>
       <c r="G15">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H15" t="s">
         <v>1</v>
@@ -891,25 +2625,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B16">
-        <v>99.208017990000002</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C16">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D16">
-        <v>5.6</v>
+        <v>5.7249999999999996</v>
       </c>
       <c r="E16">
-        <v>57</v>
+        <v>55.5</v>
       </c>
       <c r="F16">
-        <v>125.66333999999999</v>
+        <v>122.35640999999998</v>
       </c>
       <c r="G16">
-        <v>27</v>
+        <v>26.75</v>
       </c>
       <c r="H16" t="s">
         <v>1</v>
@@ -920,25 +2654,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B17">
-        <v>99.208017990000002</v>
+        <v>110.2311311</v>
       </c>
       <c r="C17">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>4.9000000000000004</v>
+        <v>5.9249999999999998</v>
       </c>
       <c r="E17">
-        <v>48</v>
+        <v>60.25</v>
       </c>
       <c r="F17">
-        <v>105.82175999999998</v>
+        <v>132.82835499999999</v>
       </c>
       <c r="G17">
-        <v>23</v>
+        <v>28.5</v>
       </c>
       <c r="H17" t="s">
         <v>1</v>
@@ -949,123 +2683,123 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B18">
-        <v>99.208017990000002</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C18">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D18">
-        <v>1.7</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="F18">
-        <v>33.069299999999998</v>
+        <v>127.86795999999998</v>
       </c>
       <c r="G18">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="H18" t="s">
         <v>1</v>
       </c>
       <c r="I18">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="B19">
-        <v>99.208017990000002</v>
+        <v>121.25424421</v>
       </c>
       <c r="C19">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>63.5</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>139.99337</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H19" t="s">
         <v>1</v>
       </c>
       <c r="I19">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>390</v>
+        <v>140</v>
       </c>
       <c r="B20">
-        <v>110.2311311</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C20">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D20">
-        <v>16.425000000000001</v>
+        <v>6.3</v>
       </c>
       <c r="E20">
-        <v>194.25</v>
+        <v>67</v>
       </c>
       <c r="F20">
-        <v>428.24743499999994</v>
+        <v>147.70953999999998</v>
       </c>
       <c r="G20">
-        <v>102.25</v>
-      </c>
-      <c r="H20">
-        <v>69.900000000000006</v>
+        <v>31</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>241</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>370</v>
+        <v>120</v>
       </c>
       <c r="B21">
-        <v>110.2311311</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D21">
-        <v>15.125</v>
+        <v>6.5750000000000002</v>
       </c>
       <c r="E21">
-        <v>170.5</v>
+        <v>66.75</v>
       </c>
       <c r="F21">
-        <v>375.88770999999997</v>
+        <v>147.15838499999998</v>
       </c>
       <c r="G21">
-        <v>91.75</v>
-      </c>
-      <c r="H21">
-        <v>72.099999999999994</v>
+        <v>31.5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>252</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>350</v>
+        <v>140</v>
       </c>
       <c r="B22">
         <v>110.2311311</v>
@@ -1074,103 +2808,103 @@
         <v>50</v>
       </c>
       <c r="D22">
-        <v>13.675000000000001</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="E22">
-        <v>139.5</v>
+        <v>71</v>
       </c>
       <c r="F22">
-        <v>307.54449</v>
+        <v>156.52802</v>
       </c>
       <c r="G22">
-        <v>81.5</v>
+        <v>33</v>
       </c>
       <c r="H22" t="s">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>264</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>330</v>
+        <v>120</v>
       </c>
       <c r="B23">
-        <v>110.2311311</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D23">
-        <v>12.85</v>
+        <v>6.9</v>
       </c>
       <c r="E23">
-        <v>127.5</v>
+        <v>70</v>
       </c>
       <c r="F23">
-        <v>281.08904999999999</v>
+        <v>154.32339999999999</v>
       </c>
       <c r="G23">
-        <v>75.25</v>
+        <v>33</v>
       </c>
       <c r="H23" t="s">
         <v>1</v>
       </c>
       <c r="I23">
-        <v>277</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>310</v>
+        <v>140</v>
       </c>
       <c r="B24">
-        <v>110.2311311</v>
+        <v>121.25424421</v>
       </c>
       <c r="C24">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D24">
-        <v>12.399999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="E24">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="F24">
-        <v>275.57749999999999</v>
+        <v>165.34649999999999</v>
       </c>
       <c r="G24">
-        <v>71.75</v>
+        <v>35</v>
       </c>
       <c r="H24" t="s">
         <v>1</v>
       </c>
       <c r="I24">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>290</v>
+        <v>160</v>
       </c>
       <c r="B25">
-        <v>110.2311311</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C25">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D25">
-        <v>11.875</v>
+        <v>7.1</v>
       </c>
       <c r="E25">
-        <v>121.75</v>
+        <v>78</v>
       </c>
       <c r="F25">
-        <v>268.412485</v>
+        <v>171.96035999999998</v>
       </c>
       <c r="G25">
-        <v>68.5</v>
+        <v>36</v>
       </c>
       <c r="H25" t="s">
         <v>1</v>
@@ -1181,25 +2915,25 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>270</v>
+        <v>140</v>
       </c>
       <c r="B26">
-        <v>110.2311311</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D26">
-        <v>11.3</v>
+        <v>7.5</v>
       </c>
       <c r="E26">
-        <v>117.75</v>
+        <v>79</v>
       </c>
       <c r="F26">
-        <v>259.59400499999998</v>
+        <v>174.16497999999999</v>
       </c>
       <c r="G26">
-        <v>63.25</v>
+        <v>37</v>
       </c>
       <c r="H26" t="s">
         <v>1</v>
@@ -1210,7 +2944,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="B27">
         <v>110.2311311</v>
@@ -1219,16 +2953,16 @@
         <v>50</v>
       </c>
       <c r="D27">
-        <v>10.675000000000001</v>
+        <v>7.5250000000000004</v>
       </c>
       <c r="E27">
-        <v>114.25</v>
+        <v>82.75</v>
       </c>
       <c r="F27">
-        <v>251.87783499999998</v>
+        <v>182.43230499999999</v>
       </c>
       <c r="G27">
-        <v>59</v>
+        <v>38.25</v>
       </c>
       <c r="H27" t="s">
         <v>1</v>
@@ -1239,25 +2973,25 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="B28">
-        <v>110.2311311</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C28">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D28">
-        <v>10.35</v>
+        <v>7.8</v>
       </c>
       <c r="E28">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="F28">
-        <v>246.91743999999997</v>
+        <v>189.59732</v>
       </c>
       <c r="G28">
-        <v>56.75</v>
+        <v>40</v>
       </c>
       <c r="H28" t="s">
         <v>1</v>
@@ -1268,25 +3002,25 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="B29">
-        <v>110.2311311</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C29">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D29">
-        <v>9.6999999999999993</v>
+        <v>7.9</v>
       </c>
       <c r="E29">
-        <v>106.75</v>
+        <v>83</v>
       </c>
       <c r="F29">
-        <v>235.34318499999998</v>
+        <v>182.98345999999998</v>
       </c>
       <c r="G29">
-        <v>52.25</v>
+        <v>39</v>
       </c>
       <c r="H29" t="s">
         <v>1</v>
@@ -1297,25 +3031,25 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="B30">
-        <v>110.2311311</v>
+        <v>121.25424421</v>
       </c>
       <c r="C30">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D30">
-        <v>9.0250000000000004</v>
+        <v>7.95</v>
       </c>
       <c r="E30">
-        <v>100.25</v>
+        <v>87.5</v>
       </c>
       <c r="F30">
-        <v>221.01315499999998</v>
+        <v>192.90424999999999</v>
       </c>
       <c r="G30">
-        <v>47.75</v>
+        <v>40.5</v>
       </c>
       <c r="H30" t="s">
         <v>1</v>
@@ -1358,22 +3092,22 @@
         <v>160</v>
       </c>
       <c r="B32">
-        <v>110.2311311</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C32">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D32">
-        <v>7.5250000000000004</v>
+        <v>8.375</v>
       </c>
       <c r="E32">
-        <v>82.75</v>
+        <v>92.25</v>
       </c>
       <c r="F32">
-        <v>182.43230499999999</v>
+        <v>203.376195</v>
       </c>
       <c r="G32">
-        <v>38.25</v>
+        <v>42.75</v>
       </c>
       <c r="H32" t="s">
         <v>1</v>
@@ -1384,25 +3118,25 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="B33">
-        <v>110.2311311</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C33">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D33">
-        <v>6.6999999999999993</v>
+        <v>8.5</v>
       </c>
       <c r="E33">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F33">
-        <v>156.52802</v>
+        <v>207.23427999999998</v>
       </c>
       <c r="G33">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="H33" t="s">
         <v>1</v>
@@ -1413,25 +3147,25 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="B34">
-        <v>110.2311311</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C34">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D34">
-        <v>5.9249999999999998</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E34">
-        <v>60.25</v>
+        <v>97</v>
       </c>
       <c r="F34">
-        <v>132.82835499999999</v>
+        <v>213.84813999999997</v>
       </c>
       <c r="G34">
-        <v>28.5</v>
+        <v>45</v>
       </c>
       <c r="H34" t="s">
         <v>1</v>
@@ -1442,25 +3176,25 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="B35">
-        <v>110.2311311</v>
+        <v>121.25424421</v>
       </c>
       <c r="C35">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D35">
-        <v>5.1750000000000007</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E35">
-        <v>50.5</v>
+        <v>97.5</v>
       </c>
       <c r="F35">
-        <v>111.33330999999998</v>
+        <v>214.95044999999999</v>
       </c>
       <c r="G35">
-        <v>24.25</v>
+        <v>45.5</v>
       </c>
       <c r="H35" t="s">
         <v>1</v>
@@ -1471,7 +3205,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="B36">
         <v>110.2311311</v>
@@ -1480,85 +3214,85 @@
         <v>50</v>
       </c>
       <c r="D36">
-        <v>1.7999999999999998</v>
+        <v>9.0250000000000004</v>
       </c>
       <c r="E36">
-        <v>15.75</v>
+        <v>100.25</v>
       </c>
       <c r="F36">
-        <v>34.722764999999995</v>
+        <v>221.01315499999998</v>
       </c>
       <c r="G36">
-        <v>7.5</v>
+        <v>47.75</v>
       </c>
       <c r="H36" t="s">
         <v>1</v>
       </c>
       <c r="I36">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="B37">
-        <v>110.2311311</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>220.46199999999999</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="H37" t="s">
         <v>1</v>
       </c>
       <c r="I37">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>390</v>
+        <v>180</v>
       </c>
       <c r="B38">
-        <v>121.25424421</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C38">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D38">
-        <v>16.75</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E38">
-        <v>184.5</v>
+        <v>103.25</v>
       </c>
       <c r="F38">
-        <v>406.75238999999999</v>
+        <v>227.62701499999997</v>
       </c>
       <c r="G38">
-        <v>103.5</v>
-      </c>
-      <c r="H38">
-        <v>72.099999999999994</v>
+        <v>48.25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>241</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>370</v>
+        <v>200</v>
       </c>
       <c r="B39">
         <v>121.25424421</v>
@@ -1567,132 +3301,132 @@
         <v>55</v>
       </c>
       <c r="D39">
-        <v>15.649999999999999</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="E39">
-        <v>167</v>
+        <v>106.5</v>
       </c>
       <c r="F39">
-        <v>368.17153999999999</v>
+        <v>234.79202999999998</v>
       </c>
       <c r="G39">
-        <v>94.5</v>
+        <v>50.5</v>
       </c>
       <c r="H39" t="s">
         <v>1</v>
       </c>
       <c r="I39">
-        <v>252</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="B40">
-        <v>121.25424421</v>
+        <v>110.2311311</v>
       </c>
       <c r="C40">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D40">
-        <v>14.45</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="E40">
-        <v>145</v>
+        <v>106.75</v>
       </c>
       <c r="F40">
-        <v>319.66989999999998</v>
+        <v>235.34318499999998</v>
       </c>
       <c r="G40">
-        <v>86</v>
+        <v>52.25</v>
       </c>
       <c r="H40" t="s">
         <v>1</v>
       </c>
       <c r="I40">
-        <v>264</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="B41">
-        <v>121.25424421</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C41">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D41">
-        <v>13.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="E41">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="F41">
-        <v>299.82831999999996</v>
+        <v>231.48509999999999</v>
       </c>
       <c r="G41">
-        <v>80.5</v>
+        <v>53</v>
       </c>
       <c r="H41" t="s">
         <v>1</v>
       </c>
       <c r="I41">
-        <v>277</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>310</v>
+        <v>180</v>
       </c>
       <c r="B42">
-        <v>121.25424421</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C42">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D42">
-        <v>13.2</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E42">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="F42">
-        <v>293.21445999999997</v>
+        <v>240.30357999999998</v>
       </c>
       <c r="G42">
-        <v>76.5</v>
+        <v>51</v>
       </c>
       <c r="H42" t="s">
         <v>1</v>
       </c>
       <c r="I42">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>290</v>
+        <v>250</v>
       </c>
       <c r="B43">
-        <v>121.25424421</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C43">
+        <v>45</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+      <c r="E43">
+        <v>107</v>
+      </c>
+      <c r="F43">
+        <v>235.89433999999997</v>
+      </c>
+      <c r="G43">
         <v>55</v>
-      </c>
-      <c r="D43">
-        <v>12.649999999999999</v>
-      </c>
-      <c r="E43">
-        <v>129.5</v>
-      </c>
-      <c r="F43">
-        <v>285.49829</v>
-      </c>
-      <c r="G43">
-        <v>73</v>
       </c>
       <c r="H43" t="s">
         <v>1</v>
@@ -1703,25 +3437,25 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>270</v>
+        <v>200</v>
       </c>
       <c r="B44">
-        <v>121.25424421</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C44">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D44">
-        <v>12</v>
+        <v>10.074999999999999</v>
       </c>
       <c r="E44">
-        <v>125.5</v>
+        <v>112.75</v>
       </c>
       <c r="F44">
-        <v>276.67980999999997</v>
+        <v>248.57090499999998</v>
       </c>
       <c r="G44">
-        <v>67.5</v>
+        <v>53.25</v>
       </c>
       <c r="H44" t="s">
         <v>1</v>
@@ -1732,7 +3466,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="B45">
         <v>121.25424421</v>
@@ -1741,16 +3475,16 @@
         <v>55</v>
       </c>
       <c r="D45">
-        <v>11.35</v>
+        <v>10.3</v>
       </c>
       <c r="E45">
-        <v>121.5</v>
+        <v>113.5</v>
       </c>
       <c r="F45">
-        <v>267.86132999999995</v>
+        <v>250.22436999999996</v>
       </c>
       <c r="G45">
-        <v>63</v>
+        <v>55.5</v>
       </c>
       <c r="H45" t="s">
         <v>1</v>
@@ -1764,22 +3498,22 @@
         <v>240</v>
       </c>
       <c r="B46">
-        <v>121.25424421</v>
+        <v>110.2311311</v>
       </c>
       <c r="C46">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D46">
-        <v>11</v>
+        <v>10.35</v>
       </c>
       <c r="E46">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F46">
-        <v>262.34977999999995</v>
+        <v>246.91743999999997</v>
       </c>
       <c r="G46">
-        <v>60.5</v>
+        <v>56.75</v>
       </c>
       <c r="H46" t="s">
         <v>1</v>
@@ -1790,25 +3524,25 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B47">
-        <v>121.25424421</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C47">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D47">
-        <v>10.3</v>
+        <v>10.6</v>
       </c>
       <c r="E47">
-        <v>113.5</v>
+        <v>119</v>
       </c>
       <c r="F47">
-        <v>250.22436999999996</v>
+        <v>262.34977999999995</v>
       </c>
       <c r="G47">
-        <v>55.5</v>
+        <v>56</v>
       </c>
       <c r="H47" t="s">
         <v>1</v>
@@ -1819,25 +3553,25 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="B48">
-        <v>121.25424421</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C48">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D48">
-        <v>9.5500000000000007</v>
+        <v>10.6</v>
       </c>
       <c r="E48">
-        <v>106.5</v>
+        <v>110</v>
       </c>
       <c r="F48">
-        <v>234.79202999999998</v>
+        <v>242.50819999999999</v>
       </c>
       <c r="G48">
-        <v>50.5</v>
+        <v>59</v>
       </c>
       <c r="H48" t="s">
         <v>1</v>
@@ -1848,25 +3582,25 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="B49">
-        <v>121.25424421</v>
+        <v>110.2311311</v>
       </c>
       <c r="C49">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D49">
-        <v>8.8000000000000007</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="E49">
-        <v>97.5</v>
+        <v>114.25</v>
       </c>
       <c r="F49">
-        <v>214.95044999999999</v>
+        <v>251.87783499999998</v>
       </c>
       <c r="G49">
-        <v>45.5</v>
+        <v>59</v>
       </c>
       <c r="H49" t="s">
         <v>1</v>
@@ -1877,25 +3611,25 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="B50">
-        <v>121.25424421</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C50">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D50">
-        <v>7.95</v>
+        <v>10.9</v>
       </c>
       <c r="E50">
-        <v>87.5</v>
+        <v>120.25</v>
       </c>
       <c r="F50">
-        <v>192.90424999999999</v>
+        <v>265.10555499999998</v>
       </c>
       <c r="G50">
-        <v>40.5</v>
+        <v>58.75</v>
       </c>
       <c r="H50" t="s">
         <v>1</v>
@@ -1906,7 +3640,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="B51">
         <v>121.25424421</v>
@@ -1915,16 +3649,16 @@
         <v>55</v>
       </c>
       <c r="D51">
-        <v>7.1</v>
+        <v>11</v>
       </c>
       <c r="E51">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="F51">
-        <v>165.34649999999999</v>
+        <v>262.34977999999995</v>
       </c>
       <c r="G51">
-        <v>35</v>
+        <v>60.5</v>
       </c>
       <c r="H51" t="s">
         <v>1</v>
@@ -1935,25 +3669,25 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>120</v>
+        <v>290</v>
       </c>
       <c r="B52">
-        <v>121.25424421</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C52">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D52">
-        <v>6.25</v>
+        <v>11.1</v>
       </c>
       <c r="E52">
-        <v>63.5</v>
+        <v>114</v>
       </c>
       <c r="F52">
-        <v>139.99337</v>
+        <v>251.32667999999998</v>
       </c>
       <c r="G52">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="H52" t="s">
         <v>1</v>
@@ -1964,25 +3698,25 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>100</v>
+        <v>270</v>
       </c>
       <c r="B53">
-        <v>121.25424421</v>
+        <v>110.2311311</v>
       </c>
       <c r="C53">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D53">
-        <v>5.45</v>
+        <v>11.3</v>
       </c>
       <c r="E53">
-        <v>53</v>
+        <v>117.75</v>
       </c>
       <c r="F53">
-        <v>116.84485999999998</v>
+        <v>259.59400499999998</v>
       </c>
       <c r="G53">
-        <v>25.5</v>
+        <v>63.25</v>
       </c>
       <c r="H53" t="s">
         <v>1</v>
@@ -1993,7 +3727,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="B54">
         <v>121.25424421</v>
@@ -2002,85 +3736,85 @@
         <v>55</v>
       </c>
       <c r="D54">
-        <v>1.9</v>
+        <v>11.35</v>
       </c>
       <c r="E54">
-        <v>16.5</v>
+        <v>121.5</v>
       </c>
       <c r="F54">
-        <v>36.37623</v>
+        <v>267.86132999999995</v>
       </c>
       <c r="G54">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="H54" t="s">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="B55">
-        <v>121.25424421</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C55">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>279.98674</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="H55" t="s">
         <v>1</v>
       </c>
       <c r="I55">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>390</v>
+        <v>310</v>
       </c>
       <c r="B56">
-        <v>132.27735731999999</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C56">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D56">
-        <v>17.074999999999999</v>
+        <v>11.6</v>
       </c>
       <c r="E56">
-        <v>174.75</v>
+        <v>117</v>
       </c>
       <c r="F56">
-        <v>385.25734499999999</v>
+        <v>257.94054</v>
       </c>
       <c r="G56">
-        <v>104.75</v>
+        <v>67</v>
       </c>
       <c r="H56" t="s">
         <v>1</v>
       </c>
       <c r="I56">
-        <v>241</v>
+        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>370</v>
+        <v>240</v>
       </c>
       <c r="B57">
         <v>132.27735731999999</v>
@@ -2089,114 +3823,114 @@
         <v>60</v>
       </c>
       <c r="D57">
-        <v>16.174999999999997</v>
+        <v>11.65</v>
       </c>
       <c r="E57">
-        <v>163.5</v>
+        <v>126</v>
       </c>
       <c r="F57">
-        <v>360.45536999999996</v>
+        <v>277.78211999999996</v>
       </c>
       <c r="G57">
-        <v>97.25</v>
+        <v>64.25</v>
       </c>
       <c r="H57" t="s">
         <v>1</v>
       </c>
       <c r="I57">
-        <v>252</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>350</v>
+        <v>290</v>
       </c>
       <c r="B58">
-        <v>132.27735731999999</v>
+        <v>110.2311311</v>
       </c>
       <c r="C58">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D58">
-        <v>15.225</v>
+        <v>11.875</v>
       </c>
       <c r="E58">
-        <v>150.5</v>
+        <v>121.75</v>
       </c>
       <c r="F58">
-        <v>331.79530999999997</v>
+        <v>268.412485</v>
       </c>
       <c r="G58">
-        <v>90.5</v>
+        <v>68.5</v>
       </c>
       <c r="H58" t="s">
         <v>1</v>
       </c>
       <c r="I58">
-        <v>264</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>330</v>
+        <v>270</v>
       </c>
       <c r="B59">
-        <v>132.27735731999999</v>
+        <v>121.25424421</v>
       </c>
       <c r="C59">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D59">
-        <v>14.55</v>
+        <v>12</v>
       </c>
       <c r="E59">
-        <v>144.5</v>
+        <v>125.5</v>
       </c>
       <c r="F59">
-        <v>318.56759</v>
+        <v>276.67980999999997</v>
       </c>
       <c r="G59">
-        <v>85.75</v>
+        <v>67.5</v>
       </c>
       <c r="H59" t="s">
         <v>1</v>
       </c>
       <c r="I59">
-        <v>277</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="B60">
-        <v>132.27735731999999</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C60">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D60">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E60">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="F60">
-        <v>310.85141999999996</v>
+        <v>262.34977999999995</v>
       </c>
       <c r="G60">
-        <v>81.25</v>
+        <v>70</v>
       </c>
       <c r="H60" t="s">
         <v>1</v>
       </c>
       <c r="I60">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>290</v>
+        <v>250</v>
       </c>
       <c r="B61">
         <v>132.27735731999999</v>
@@ -2205,16 +3939,16 @@
         <v>60</v>
       </c>
       <c r="D61">
-        <v>13.424999999999999</v>
+        <v>12.024999999999999</v>
       </c>
       <c r="E61">
-        <v>137.25</v>
+        <v>128.75</v>
       </c>
       <c r="F61">
-        <v>302.58409499999999</v>
+        <v>283.84482499999996</v>
       </c>
       <c r="G61">
-        <v>77.5</v>
+        <v>67</v>
       </c>
       <c r="H61" t="s">
         <v>1</v>
@@ -2225,25 +3959,25 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="B62">
-        <v>132.27735731999999</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C62">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D62">
-        <v>12.7</v>
+        <v>12.3</v>
       </c>
       <c r="E62">
-        <v>133.25</v>
+        <v>133</v>
       </c>
       <c r="F62">
-        <v>293.76561499999997</v>
+        <v>293.21445999999997</v>
       </c>
       <c r="G62">
-        <v>71.75</v>
+        <v>68</v>
       </c>
       <c r="H62" t="s">
         <v>1</v>
@@ -2254,54 +3988,54 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>250</v>
+        <v>310</v>
       </c>
       <c r="B63">
-        <v>132.27735731999999</v>
+        <v>110.2311311</v>
       </c>
       <c r="C63">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D63">
-        <v>12.024999999999999</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="E63">
-        <v>128.75</v>
+        <v>125</v>
       </c>
       <c r="F63">
-        <v>283.84482499999996</v>
+        <v>275.57749999999999</v>
       </c>
       <c r="G63">
-        <v>67</v>
+        <v>71.75</v>
       </c>
       <c r="H63" t="s">
         <v>1</v>
       </c>
       <c r="I63">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>240</v>
+        <v>290</v>
       </c>
       <c r="B64">
-        <v>132.27735731999999</v>
+        <v>121.25424421</v>
       </c>
       <c r="C64">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D64">
-        <v>11.65</v>
+        <v>12.649999999999999</v>
       </c>
       <c r="E64">
-        <v>126</v>
+        <v>129.5</v>
       </c>
       <c r="F64">
-        <v>277.78211999999996</v>
+        <v>285.49829</v>
       </c>
       <c r="G64">
-        <v>64.25</v>
+        <v>73</v>
       </c>
       <c r="H64" t="s">
         <v>1</v>
@@ -2312,25 +4046,25 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="B65">
-        <v>132.27735731999999</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C65">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D65">
-        <v>10.9</v>
+        <v>12.7</v>
       </c>
       <c r="E65">
-        <v>120.25</v>
+        <v>136</v>
       </c>
       <c r="F65">
-        <v>265.10555499999998</v>
+        <v>299.82831999999996</v>
       </c>
       <c r="G65">
-        <v>58.75</v>
+        <v>71</v>
       </c>
       <c r="H65" t="s">
         <v>1</v>
@@ -2341,7 +4075,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="B66">
         <v>132.27735731999999</v>
@@ -2350,16 +4084,16 @@
         <v>60</v>
       </c>
       <c r="D66">
-        <v>10.074999999999999</v>
+        <v>12.7</v>
       </c>
       <c r="E66">
-        <v>112.75</v>
+        <v>133.25</v>
       </c>
       <c r="F66">
-        <v>248.57090499999998</v>
+        <v>293.76561499999997</v>
       </c>
       <c r="G66">
-        <v>53.25</v>
+        <v>71.75</v>
       </c>
       <c r="H66" t="s">
         <v>1</v>
@@ -2370,112 +4104,112 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>180</v>
+        <v>330</v>
       </c>
       <c r="B67">
-        <v>132.27735731999999</v>
+        <v>110.2311311</v>
       </c>
       <c r="C67">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D67">
-        <v>9.3000000000000007</v>
+        <v>12.85</v>
       </c>
       <c r="E67">
-        <v>103.25</v>
+        <v>127.5</v>
       </c>
       <c r="F67">
-        <v>227.62701499999997</v>
+        <v>281.08904999999999</v>
       </c>
       <c r="G67">
-        <v>48.25</v>
+        <v>75.25</v>
       </c>
       <c r="H67" t="s">
         <v>1</v>
       </c>
       <c r="I67">
-        <v>300</v>
+        <v>277</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>160</v>
+        <v>350</v>
       </c>
       <c r="B68">
-        <v>132.27735731999999</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C68">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D68">
-        <v>8.375</v>
+        <v>12.9</v>
       </c>
       <c r="E68">
-        <v>92.25</v>
+        <v>134</v>
       </c>
       <c r="F68">
-        <v>203.376195</v>
+        <v>295.41907999999995</v>
       </c>
       <c r="G68">
-        <v>42.75</v>
-      </c>
-      <c r="H68" t="s">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="H68">
+        <v>72.099999999999994</v>
       </c>
       <c r="I68">
-        <v>300</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>140</v>
+        <v>310</v>
       </c>
       <c r="B69">
-        <v>132.27735731999999</v>
+        <v>121.25424421</v>
       </c>
       <c r="C69">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D69">
-        <v>7.5</v>
+        <v>13.2</v>
       </c>
       <c r="E69">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="F69">
-        <v>174.16497999999999</v>
+        <v>293.21445999999997</v>
       </c>
       <c r="G69">
-        <v>37</v>
+        <v>76.5</v>
       </c>
       <c r="H69" t="s">
         <v>1</v>
       </c>
       <c r="I69">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>120</v>
+        <v>270</v>
       </c>
       <c r="B70">
-        <v>132.27735731999999</v>
+        <v>143.30047042999999</v>
       </c>
       <c r="C70">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D70">
-        <v>6.5750000000000002</v>
+        <v>13.4</v>
       </c>
       <c r="E70">
-        <v>66.75</v>
+        <v>141</v>
       </c>
       <c r="F70">
-        <v>147.15838499999998</v>
+        <v>310.85141999999996</v>
       </c>
       <c r="G70">
-        <v>31.5</v>
+        <v>76</v>
       </c>
       <c r="H70" t="s">
         <v>1</v>
@@ -2486,7 +4220,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>100</v>
+        <v>290</v>
       </c>
       <c r="B71">
         <v>132.27735731999999</v>
@@ -2495,16 +4229,16 @@
         <v>60</v>
       </c>
       <c r="D71">
-        <v>5.7249999999999996</v>
+        <v>13.424999999999999</v>
       </c>
       <c r="E71">
-        <v>55.5</v>
+        <v>137.25</v>
       </c>
       <c r="F71">
-        <v>122.35640999999998</v>
+        <v>302.58409499999999</v>
       </c>
       <c r="G71">
-        <v>26.75</v>
+        <v>77.5</v>
       </c>
       <c r="H71" t="s">
         <v>1</v>
@@ -2515,94 +4249,94 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
+        <v>350</v>
+      </c>
+      <c r="B72">
+        <v>110.2311311</v>
+      </c>
+      <c r="C72">
         <v>50</v>
       </c>
-      <c r="B72">
-        <v>132.27735731999999</v>
-      </c>
-      <c r="C72">
-        <v>60</v>
-      </c>
       <c r="D72">
-        <v>2</v>
+        <v>13.675000000000001</v>
       </c>
       <c r="E72">
-        <v>17.25</v>
+        <v>139.5</v>
       </c>
       <c r="F72">
-        <v>38.029694999999997</v>
+        <v>307.54449</v>
       </c>
       <c r="G72">
-        <v>8.5</v>
+        <v>81.5</v>
       </c>
       <c r="H72" t="s">
         <v>1</v>
       </c>
       <c r="I72">
-        <v>250</v>
+        <v>264</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>15</v>
+        <v>330</v>
       </c>
       <c r="B73">
-        <v>132.27735731999999</v>
+        <v>121.25424421</v>
       </c>
       <c r="C73">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>13.7</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>299.82831999999996</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>80.5</v>
       </c>
       <c r="H73" t="s">
         <v>1</v>
       </c>
       <c r="I73">
-        <v>250</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>390</v>
+        <v>310</v>
       </c>
       <c r="B74">
-        <v>143.30047042999999</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C74">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D74">
-        <v>17.399999999999999</v>
+        <v>14</v>
       </c>
       <c r="E74">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="F74">
-        <v>363.76229999999998</v>
+        <v>310.85141999999996</v>
       </c>
       <c r="G74">
-        <v>106</v>
+        <v>81.25</v>
       </c>
       <c r="H74" t="s">
         <v>1</v>
       </c>
       <c r="I74">
-        <v>241</v>
+        <v>289</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>370</v>
+        <v>290</v>
       </c>
       <c r="B75">
         <v>143.30047042999999</v>
@@ -2611,22 +4345,22 @@
         <v>65</v>
       </c>
       <c r="D75">
-        <v>16.7</v>
+        <v>14.2</v>
       </c>
       <c r="E75">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="F75">
-        <v>352.73919999999998</v>
+        <v>319.66989999999998</v>
       </c>
       <c r="G75">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="H75" t="s">
         <v>1</v>
       </c>
       <c r="I75">
-        <v>252</v>
+        <v>300</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -2634,22 +4368,22 @@
         <v>350</v>
       </c>
       <c r="B76">
-        <v>143.30047042999999</v>
+        <v>121.25424421</v>
       </c>
       <c r="C76">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D76">
-        <v>16</v>
+        <v>14.45</v>
       </c>
       <c r="E76">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="F76">
-        <v>343.92071999999996</v>
+        <v>319.66989999999998</v>
       </c>
       <c r="G76">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H76" t="s">
         <v>1</v>
@@ -2663,22 +4397,22 @@
         <v>330</v>
       </c>
       <c r="B77">
-        <v>143.30047042999999</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C77">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D77">
-        <v>15.4</v>
+        <v>14.55</v>
       </c>
       <c r="E77">
-        <v>153</v>
+        <v>144.5</v>
       </c>
       <c r="F77">
-        <v>337.30685999999997</v>
+        <v>318.56759</v>
       </c>
       <c r="G77">
-        <v>91</v>
+        <v>85.75</v>
       </c>
       <c r="H77" t="s">
         <v>1</v>
@@ -2689,36 +4423,36 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>310</v>
+        <v>370</v>
       </c>
       <c r="B78">
-        <v>143.30047042999999</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C78">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D78">
-        <v>14.8</v>
+        <v>14.6</v>
       </c>
       <c r="E78">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="F78">
-        <v>328.48837999999995</v>
+        <v>383.60387999999995</v>
       </c>
       <c r="G78">
-        <v>86</v>
-      </c>
-      <c r="H78" t="s">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="H78">
+        <v>69.900000000000006</v>
       </c>
       <c r="I78">
-        <v>289</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B79">
         <v>143.30047042999999</v>
@@ -2727,85 +4461,85 @@
         <v>65</v>
       </c>
       <c r="D79">
-        <v>14.2</v>
+        <v>14.8</v>
       </c>
       <c r="E79">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F79">
-        <v>319.66989999999998</v>
+        <v>328.48837999999995</v>
       </c>
       <c r="G79">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H79" t="s">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>270</v>
+        <v>370</v>
       </c>
       <c r="B80">
-        <v>143.30047042999999</v>
+        <v>110.2311311</v>
       </c>
       <c r="C80">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D80">
-        <v>13.4</v>
+        <v>15.125</v>
       </c>
       <c r="E80">
-        <v>141</v>
+        <v>170.5</v>
       </c>
       <c r="F80">
-        <v>310.85141999999996</v>
+        <v>375.88770999999997</v>
       </c>
       <c r="G80">
-        <v>76</v>
-      </c>
-      <c r="H80" t="s">
-        <v>1</v>
+        <v>91.75</v>
+      </c>
+      <c r="H80">
+        <v>72.099999999999994</v>
       </c>
       <c r="I80">
-        <v>300</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="B81">
-        <v>143.30047042999999</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C81">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D81">
-        <v>12.7</v>
+        <v>15.225</v>
       </c>
       <c r="E81">
-        <v>136</v>
+        <v>150.5</v>
       </c>
       <c r="F81">
-        <v>299.82831999999996</v>
+        <v>331.79530999999997</v>
       </c>
       <c r="G81">
-        <v>71</v>
+        <v>90.5</v>
       </c>
       <c r="H81" t="s">
         <v>1</v>
       </c>
       <c r="I81">
-        <v>300</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="B82">
         <v>143.30047042999999</v>
@@ -2814,56 +4548,56 @@
         <v>65</v>
       </c>
       <c r="D82">
-        <v>12.3</v>
+        <v>15.4</v>
       </c>
       <c r="E82">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="F82">
-        <v>293.21445999999997</v>
+        <v>337.30685999999997</v>
       </c>
       <c r="G82">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="H82" t="s">
         <v>1</v>
       </c>
       <c r="I82">
-        <v>300</v>
+        <v>277</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>220</v>
+        <v>370</v>
       </c>
       <c r="B83">
-        <v>143.30047042999999</v>
+        <v>121.25424421</v>
       </c>
       <c r="C83">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D83">
-        <v>11.5</v>
+        <v>15.649999999999999</v>
       </c>
       <c r="E83">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="F83">
-        <v>279.98674</v>
+        <v>368.17153999999999</v>
       </c>
       <c r="G83">
-        <v>62</v>
+        <v>94.5</v>
       </c>
       <c r="H83" t="s">
         <v>1</v>
       </c>
       <c r="I83">
-        <v>300</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="B84">
         <v>143.30047042999999</v>
@@ -2872,114 +4606,114 @@
         <v>65</v>
       </c>
       <c r="D84">
-        <v>10.6</v>
+        <v>16</v>
       </c>
       <c r="E84">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="F84">
-        <v>262.34977999999995</v>
+        <v>343.92071999999996</v>
       </c>
       <c r="G84">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="H84" t="s">
         <v>1</v>
       </c>
       <c r="I84">
-        <v>300</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>180</v>
+        <v>390</v>
       </c>
       <c r="B85">
-        <v>143.30047042999999</v>
+        <v>99.208017990000002</v>
       </c>
       <c r="C85">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D85">
-        <v>9.8000000000000007</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="E85">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="F85">
-        <v>240.30357999999998</v>
+        <v>449.74247999999994</v>
       </c>
       <c r="G85">
-        <v>51</v>
-      </c>
-      <c r="H85" t="s">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="H85">
+        <v>68.8</v>
       </c>
       <c r="I85">
-        <v>300</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>160</v>
+        <v>370</v>
       </c>
       <c r="B86">
-        <v>143.30047042999999</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C86">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D86">
-        <v>8.8000000000000007</v>
+        <v>16.174999999999997</v>
       </c>
       <c r="E86">
-        <v>97</v>
+        <v>163.5</v>
       </c>
       <c r="F86">
-        <v>213.84813999999997</v>
+        <v>360.45536999999996</v>
       </c>
       <c r="G86">
-        <v>45</v>
+        <v>97.25</v>
       </c>
       <c r="H86" t="s">
         <v>1</v>
       </c>
       <c r="I86">
-        <v>300</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>140</v>
+        <v>390</v>
       </c>
       <c r="B87">
-        <v>143.30047042999999</v>
+        <v>110.2311311</v>
       </c>
       <c r="C87">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D87">
-        <v>7.9</v>
+        <v>16.425000000000001</v>
       </c>
       <c r="E87">
-        <v>83</v>
+        <v>194.25</v>
       </c>
       <c r="F87">
-        <v>182.98345999999998</v>
+        <v>428.24743499999994</v>
       </c>
       <c r="G87">
-        <v>39</v>
-      </c>
-      <c r="H87" t="s">
-        <v>1</v>
+        <v>102.25</v>
+      </c>
+      <c r="H87">
+        <v>69.900000000000006</v>
       </c>
       <c r="I87">
-        <v>300</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>120</v>
+        <v>370</v>
       </c>
       <c r="B88">
         <v>143.30047042999999</v>
@@ -2988,85 +4722,85 @@
         <v>65</v>
       </c>
       <c r="D88">
-        <v>6.9</v>
+        <v>16.7</v>
       </c>
       <c r="E88">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="F88">
-        <v>154.32339999999999</v>
+        <v>352.73919999999998</v>
       </c>
       <c r="G88">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="H88" t="s">
         <v>1</v>
       </c>
       <c r="I88">
-        <v>300</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>100</v>
+        <v>390</v>
       </c>
       <c r="B89">
-        <v>143.30047042999999</v>
+        <v>121.25424421</v>
       </c>
       <c r="C89">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D89">
-        <v>6</v>
+        <v>16.75</v>
       </c>
       <c r="E89">
-        <v>58</v>
+        <v>184.5</v>
       </c>
       <c r="F89">
-        <v>127.86795999999998</v>
+        <v>406.75238999999999</v>
       </c>
       <c r="G89">
-        <v>28</v>
-      </c>
-      <c r="H89" t="s">
-        <v>1</v>
+        <v>103.5</v>
+      </c>
+      <c r="H89">
+        <v>72.099999999999994</v>
       </c>
       <c r="I89">
-        <v>300</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>50</v>
+        <v>390</v>
       </c>
       <c r="B90">
-        <v>143.30047042999999</v>
+        <v>132.27735731999999</v>
       </c>
       <c r="C90">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D90">
-        <v>2.1</v>
+        <v>17.074999999999999</v>
       </c>
       <c r="E90">
-        <v>18</v>
+        <v>174.75</v>
       </c>
       <c r="F90">
-        <v>39.683159999999994</v>
+        <v>385.25734499999999</v>
       </c>
       <c r="G90">
-        <v>9</v>
+        <v>104.75</v>
       </c>
       <c r="H90" t="s">
         <v>1</v>
       </c>
       <c r="I90">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>15</v>
+        <v>390</v>
       </c>
       <c r="B91">
         <v>143.30047042999999</v>
@@ -3075,25 +4809,28 @@
         <v>65</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>363.76229999999998</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="H91" t="s">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I92">
+    <sortCondition ref="D1:D92"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>